<commit_message>
Add courses and resources
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laleakarun/Desktop/spring_2024/PILAB/boun-pilab.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20233DD7-2A89-1340-BAEA-41987AC09A0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A906499-A1E5-7340-A760-701044C061D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="4" xr2:uid="{04359DB9-1351-624C-B0E4-66C5D109ADF1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{04359DB9-1351-624C-B0E4-66C5D109ADF1}"/>
   </bookViews>
   <sheets>
     <sheet name="faculty" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="79">
   <si>
     <t>faculty_member</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Lale Akarun</t>
   </si>
   <si>
-    <t>akarun at boun.edu.tr</t>
-  </si>
-  <si>
     <t>BM 28</t>
   </si>
   <si>
@@ -74,12 +71,6 @@
     <t>Berk Gökberk</t>
   </si>
   <si>
-    <t>inci.baytas at boun.edu.tr</t>
-  </si>
-  <si>
-    <t>berk.gokberk at boun.edu.tr</t>
-  </si>
-  <si>
     <t>BM 24</t>
   </si>
   <si>
@@ -182,66 +173,12 @@
     <t>https://www.cmpe.boun.edu.tr/tr/courses/cmpe532</t>
   </si>
   <si>
-    <t>CmpE 510</t>
-  </si>
-  <si>
-    <t>Machine Translation</t>
-  </si>
-  <si>
-    <t>Tunga Güngör</t>
-  </si>
-  <si>
-    <t>https://www.cmpe.boun.edu.tr/courses/cmpe510</t>
-  </si>
-  <si>
-    <t>https://www.cmpe.boun.edu.tr/node/20579</t>
-  </si>
-  <si>
-    <t>CmpE 549</t>
-  </si>
-  <si>
-    <t>Bioinformatics</t>
-  </si>
-  <si>
-    <t>Arzucan Özgür</t>
-  </si>
-  <si>
-    <t>CmpE 493</t>
-  </si>
-  <si>
-    <t>Introduction to Information Retrieval</t>
-  </si>
-  <si>
-    <t>https://www.cmpe.boun.edu.tr/tr/courses/cmpe493</t>
-  </si>
-  <si>
-    <t>CmpE 58T</t>
-  </si>
-  <si>
-    <t>https://www.cmpe.boun.edu.tr/tr/courses/cmpe58t</t>
-  </si>
-  <si>
     <t>CmpE 597</t>
   </si>
   <si>
-    <t>Deep Lerning</t>
-  </si>
-  <si>
     <t>https://www.cmpe.boun.edu.tr/courses/cmpe597</t>
   </si>
   <si>
-    <t>CmpE 561</t>
-  </si>
-  <si>
-    <t>Natural Language Processing</t>
-  </si>
-  <si>
-    <t>Advanced Natural Language Processing</t>
-  </si>
-  <si>
-    <t>https://www.cmpe.boun.edu.tr/courses/cmpe561</t>
-  </si>
-  <si>
     <t>CmpE 537</t>
   </si>
   <si>
@@ -249,13 +186,94 @@
   </si>
   <si>
     <t>https://www.cmpe.boun.edu.tr/tr/courses/cmpe537</t>
+  </si>
+  <si>
+    <t>CmpE 538</t>
+  </si>
+  <si>
+    <t>3D Computer Vision</t>
+  </si>
+  <si>
+    <t>https://www.cmpe.boun.edu.tr/tr/courses/cmpe538</t>
+  </si>
+  <si>
+    <t>CmpE 593</t>
+  </si>
+  <si>
+    <t>Deep Learning for Computer Vision</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Deep Learning</t>
+  </si>
+  <si>
+    <t>CmpE 462</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>https://www.cmpe.boun.edu.tr/courses/cmpe462</t>
+  </si>
+  <si>
+    <t>CmpE 544</t>
+  </si>
+  <si>
+    <t>Pattern Recognition</t>
+  </si>
+  <si>
+    <t>https://www.cmpe.boun.edu.tr/courses/cmpe544</t>
+  </si>
+  <si>
+    <t>CmpE 496</t>
+  </si>
+  <si>
+    <t>Cmpe 530</t>
+  </si>
+  <si>
+    <t>Mathematical Fundamentals of Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>https://www.cmpe.boun.edu.tr/courses/cmpe530</t>
+  </si>
+  <si>
+    <t>Introduction to Computer Graphics</t>
+  </si>
+  <si>
+    <t>https://www.cmpe.boun.edu.tr/courses/cmpe460</t>
+  </si>
+  <si>
+    <t>gurgen a bogazici.edu.tr</t>
+  </si>
+  <si>
+    <t>berk.gokberk at bogazici.edu.tr</t>
+  </si>
+  <si>
+    <t>inci.baytas at bogazici.edu.tr</t>
+  </si>
+  <si>
+    <t>akarun at bogazici.edu.tr</t>
+  </si>
+  <si>
+    <t>BM 23</t>
+  </si>
+  <si>
+    <t>+90 212 358 1500</t>
+  </si>
+  <si>
+    <t>http://www.cmpe.boun.edu.tr/~gurgen</t>
+  </si>
+  <si>
+    <t>fikret_gurgen.jpeg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -267,6 +285,19 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -293,10 +324,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -612,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02F147BE-FC57-3245-A0D4-D84382FAE310}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,59 +686,79 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -730,51 +783,51 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -801,15 +854,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -817,10 +870,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -845,40 +898,40 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -888,10 +941,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E6E818-0D90-3146-A9BF-80CF463AF58E}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -904,55 +957,55 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>54</v>
@@ -960,19 +1013,36 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>60</v>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{32184F64-5B0B-6D4E-8214-90F3A204FA6E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -995,80 +1065,77 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{502FA7C1-D50D-944B-B97D-AD16C675F824}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{568C5270-A20C-9F41-ACBB-A635AA40673C}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{686097B7-057A-2748-A52C-CC869B2DDCD0}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{F3BE17A4-079F-E04B-8312-829B2F123BEC}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{568C5270-A20C-9F41-ACBB-A635AA40673C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>